<commit_message>
Finale output and results
</commit_message>
<xml_diff>
--- a/Admin/Invoices/Manual testcases/Pending Invoice.xlsx
+++ b/Admin/Invoices/Manual testcases/Pending Invoice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sprint124\zm-buyerautomation\Admin\Invoices\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9934AF-CD35-40BF-913E-AF67291B2BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB664FC2-F625-4B89-AFA4-E850FE70DEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>SL. No</t>
   </si>
@@ -432,9 +432,6 @@
     <t>Once click the 'Reject' it appears dialog of Reject selected files screen</t>
   </si>
   <si>
-    <t>It should display the New list of :                                                    *Non-food invoice                                                                                  *Image not clear/cut off - please retake                                                       *Duplicate image upload - no action required                                 *Wrong outlet/section                                                                       *Missing page                                                                                      *Others (Please specify)</t>
-  </si>
-  <si>
     <t>Confirm rejection and X icon</t>
   </si>
   <si>
@@ -493,6 +490,9 @@
   </si>
   <si>
     <t>It redirected to main page</t>
+  </si>
+  <si>
+    <t>It should display the New list of :                                                    *Non-food invoice                                                                                  *Image not clear/cut off - please retake                                                       *Duplicate image upload - no action required                                 *Wrong outlet/section                                                                       *Missing page                                                                                      *Others (Please specify) and Type up to 40 characters</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -613,14 +613,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -905,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1173,7 +1166,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="10">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1191,12 +1184,12 @@
       <c r="F12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="10">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1214,12 +1207,12 @@
       <c r="F13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="110" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="10">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1235,11 +1228,14 @@
         <v>44</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>45</v>
+        <v>53</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="37" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1252,14 +1248,17 @@
         <v>43</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1269,20 +1268,20 @@
         <v>19</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1292,15 +1291,15 @@
         <v>19</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="9" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>